<commit_message>
Additional changes to start on VT data
</commit_message>
<xml_diff>
--- a/IO_M1_new/Reprod_RunControl_M1_new.xlsx
+++ b/IO_M1_new/Reprod_RunControl_M1_new.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="364">
   <si>
     <t xml:space="preserve">Sheet #</t>
   </si>
@@ -710,6 +710,18 @@
   </si>
   <si>
     <t xml:space="preserve">75% initial Funding; open 30-year cp; 5-year asset smoothing, DR 7.5%, ir 8.22%, sd 12%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSERS_A1F075_O30pA5_a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSERS-6.fillin.yos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSERS-6.fillin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSERS.yos</t>
   </si>
   <si>
     <t xml:space="preserve">duration</t>
@@ -1628,7 +1640,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.60728744939271"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3522267206478"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1827,42 +1839,42 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AY47"/>
+  <dimension ref="A1:AY49"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="C28" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+      <selection pane="topRight" activeCell="A49" activeCellId="0" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.7408906882591"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.0647773279352"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="4" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.995951417004"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="true" max="10" min="9" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="22.8178137651822"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="4" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="21" min="17" style="0" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="26" min="25" style="0" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="29" min="27" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="29" min="27" style="0" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="30" min="30" style="0" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="36" min="32" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="36" min="32" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="12.5344129554656"/>
     <col collapsed="false" hidden="false" max="41" min="38" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="43" min="42" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="44" min="44" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="48" min="45" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="48" min="45" style="0" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="51" min="49" style="4" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="52" style="0" width="8.57085020242915"/>
   </cols>
@@ -2309,7 +2321,7 @@
         <v>141</v>
       </c>
       <c r="C7" s="28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -2469,8 +2481,7 @@
         <v>158</v>
       </c>
       <c r="C8" s="28" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -2630,8 +2641,7 @@
         <v>160</v>
       </c>
       <c r="C9" s="28" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -2791,8 +2801,7 @@
         <v>162</v>
       </c>
       <c r="C10" s="28" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -2952,8 +2961,7 @@
         <v>165</v>
       </c>
       <c r="C11" s="28" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -3113,8 +3121,7 @@
         <v>167</v>
       </c>
       <c r="C12" s="28" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -3274,7 +3281,7 @@
         <v>169</v>
       </c>
       <c r="C13" s="28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -3434,8 +3441,7 @@
         <v>172</v>
       </c>
       <c r="C14" s="28" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -3595,8 +3601,7 @@
         <v>174</v>
       </c>
       <c r="C15" s="28" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -3756,8 +3761,7 @@
         <v>176</v>
       </c>
       <c r="C16" s="28" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -3917,8 +3921,7 @@
         <v>178</v>
       </c>
       <c r="C17" s="28" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -4107,7 +4110,7 @@
         <v>180</v>
       </c>
       <c r="C19" s="28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -4267,7 +4270,7 @@
         <v>183</v>
       </c>
       <c r="C20" s="28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -4427,8 +4430,7 @@
         <v>185</v>
       </c>
       <c r="C21" s="28" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -4588,7 +4590,7 @@
         <v>187</v>
       </c>
       <c r="C22" s="28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -4748,8 +4750,7 @@
         <v>189</v>
       </c>
       <c r="C23" s="28" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -4909,7 +4910,7 @@
         <v>191</v>
       </c>
       <c r="C24" s="28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -5069,7 +5070,7 @@
         <v>193</v>
       </c>
       <c r="C25" s="28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -5257,7 +5258,7 @@
         <v>195</v>
       </c>
       <c r="C27" s="28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -5418,7 +5419,7 @@
         <v>197</v>
       </c>
       <c r="C28" s="28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -5579,7 +5580,7 @@
         <v>197</v>
       </c>
       <c r="C29" s="28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -5740,8 +5741,7 @@
         <v>200</v>
       </c>
       <c r="C30" s="28" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -5902,7 +5902,7 @@
         <v>202</v>
       </c>
       <c r="C31" s="28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -6063,7 +6063,7 @@
         <v>204</v>
       </c>
       <c r="C32" s="28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -6254,8 +6254,7 @@
         <v>193</v>
       </c>
       <c r="C34" s="28" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -6415,7 +6414,7 @@
         <v>195</v>
       </c>
       <c r="C35" s="28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D35" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -6576,7 +6575,7 @@
         <v>200</v>
       </c>
       <c r="C36" s="28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D36" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -6796,7 +6795,7 @@
         <v>211</v>
       </c>
       <c r="C39" s="28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D39" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -6956,7 +6955,7 @@
         <v>214</v>
       </c>
       <c r="C40" s="28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -7116,7 +7115,7 @@
         <v>216</v>
       </c>
       <c r="C41" s="28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D41" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -7276,7 +7275,7 @@
         <v>218</v>
       </c>
       <c r="C42" s="28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D42" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -7436,7 +7435,7 @@
         <v>220</v>
       </c>
       <c r="C43" s="28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D43" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -7656,7 +7655,7 @@
         <v>223</v>
       </c>
       <c r="C46" s="28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -7816,7 +7815,7 @@
         <v>225</v>
       </c>
       <c r="C47" s="28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D47" s="28" t="n">
         <f aca="false">FALSE()</f>
@@ -7964,6 +7963,166 @@
         <v>1</v>
       </c>
       <c r="AY47" s="28" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="B49" s="31" t="s">
+        <v>216</v>
+      </c>
+      <c r="C49" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" s="28" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="G49" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H49" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="K49" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="L49" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="M49" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="N49" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="O49" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="P49" s="28" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="Q49" s="27" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="R49" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="S49" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="T49" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="U49" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="V49" s="27" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="W49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X49" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y49" s="27" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="Z49" s="27" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="AA49" s="27" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AB49" s="27" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AC49" s="27" t="n">
+        <v>0.075</v>
+      </c>
+      <c r="AD49" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="AE49" s="5" t="n">
+        <v>0.0822</v>
+      </c>
+      <c r="AF49" s="27" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="AG49" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="AH49" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="AI49" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="AJ49" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK49" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="AL49" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM49" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="AN49" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="AO49" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP49" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="AQ49" s="29" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="AR49" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="AS49" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="AT49" s="30" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="AU49" s="30" t="n">
+        <v>0.145</v>
+      </c>
+      <c r="AV49" s="30" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AW49" s="28" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="AX49" s="28" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="AY49" s="28" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -7983,87 +8142,87 @@
     <mergeCell ref="AS4:AV4"/>
   </mergeCells>
   <dataValidations count="21">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AN6:AN47" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AN6:AN47 AN49" type="list">
       <formula1>"MA,EAA"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AI6:AI47" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AI6:AI47 AI49" type="list">
       <formula1>"cd,cp,sl"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AH6:AH47" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AH6:AH47 AH49" type="list">
       <formula1>"open,closed"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AS6:AS47" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AS6:AS47 AS49" type="list">
       <formula1>ConPolicy</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="P6:P47" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="P6:P47 P49" type="list">
       <formula1>"TRUE,FALSE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Decimal, 0-10% please" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="V6:V47 AB6:AB47" type="decimal">
+    <dataValidation allowBlank="true" operator="between" prompt="Decimal, 0-10% please" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="V6:V47 AB6:AB47 V49 AB49" type="decimal">
       <formula1>0</formula1>
       <formula2>0.1</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Integer, 0-15" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="W6:X47" type="whole">
+    <dataValidation allowBlank="true" operator="between" prompt="Integer, 0-15" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="W6:X47 W49:X49" type="whole">
       <formula1>0</formula1>
       <formula2>15</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Decimal, 0-20% please" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Y6:AA47 AC6:AC47 AE6:AE47" type="decimal">
+    <dataValidation allowBlank="true" operator="between" prompt="Decimal, 0-20% please" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Y6:AA47 AC6:AC47 AE6:AE47 Y49:AA49 AC49 AE49" type="decimal">
       <formula1>0</formula1>
       <formula2>0.2</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Integer, 0 to 30, please" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AJ6:AJ47" type="whole">
+    <dataValidation allowBlank="true" operator="between" prompt="Integer, 0 to 30, please" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AJ6:AJ47 AJ49" type="whole">
       <formula1>0</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Decimal, 0-75%" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AT6:AU47" type="decimal">
+    <dataValidation allowBlank="true" operator="between" prompt="Decimal, 0-75%" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AT6:AU47 AT49:AU49" type="decimal">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Decimal, 0-30%" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AV6:AV47" type="decimal">
+    <dataValidation allowBlank="true" operator="between" prompt="Decimal, 0-30%" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AV6:AV47 AV49" type="decimal">
       <formula1>0</formula1>
       <formula2>0.3</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Decimal, 0-75% please" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AF6:AF47" type="decimal">
+    <dataValidation allowBlank="true" operator="between" prompt="Decimal, 0-75% please" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AF6:AF47 AF49" type="decimal">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Integer, 1 to 30" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AL6:AL47" type="whole">
+    <dataValidation allowBlank="true" operator="between" prompt="Integer, 1 to 30" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AL6:AL47 AL49" type="whole">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AM6:AM47" type="decimal">
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AM6:AM47 AM49" type="decimal">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="lessThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AO6:AO47" type="decimal">
+    <dataValidation allowBlank="true" operator="lessThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AO6:AO47 AO49" type="decimal">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Decimal, 0-20% please" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AD6:AD47" type="none">
+    <dataValidation allowBlank="true" operator="between" prompt="Decimal, 0-20% please" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AD6:AD47 AD49" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AW6:AY47 C7:D17 C19:D25 C27:D32 C34:D36 C39:D43 C46:D47" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AW6:AY47 C7:D17 C19:D25 C27:D32 C34:D36 C39:D43 C46:D47 C49:D49 AW49:AY49" type="list">
       <formula1>"TRUE,FALSE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AP6:AP47" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AP6:AP47 AP49" type="list">
       <formula1>"MA,AL,AL_pct"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AQ6:AQ47" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AQ6:AQ47 AQ49" type="decimal">
       <formula1>0</formula1>
       <formula2>1.5</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Integer 55 to 65, please" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="S6:S47" type="whole">
+    <dataValidation allowBlank="true" operator="between" prompt="Integer 55 to 65, please" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="S6:S47 S49" type="whole">
       <formula1>35</formula1>
       <formula2>80</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I6:J47" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I6:J47 I49:J49" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -8083,15 +8242,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:D13"/>
+  <dimension ref="A3:D15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1012145748988"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8106,7 +8265,7 @@
         <v>119</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8249,13 +8408,41 @@
         <v>59</v>
       </c>
     </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="B14" s="27" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="C14" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="B15" s="27" t="n">
+        <v>0.0822</v>
+      </c>
+      <c r="C15" s="27" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="between" prompt="Decimal, 0-75% please" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4:C13" type="decimal">
+    <dataValidation allowBlank="true" operator="between" prompt="Decimal, 0-75% please" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4:C15" type="decimal">
       <formula1>0</formula1>
       <formula2>-PS5</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Decimal, 0-20% please" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B4:B13" type="decimal">
+    <dataValidation allowBlank="true" operator="between" prompt="Decimal, 0-20% please" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B4:B15" type="decimal">
       <formula1>-1</formula1>
       <formula2>0.5</formula2>
     </dataValidation>
@@ -8291,13 +8478,13 @@
         <v>88</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -8318,7 +8505,7 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -8329,30 +8516,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8375,7 +8562,7 @@
         <v>20</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -8402,15 +8589,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5303643724696"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.03643724696356"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="89.336032388664"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="90.085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="36" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="B1" s="36"/>
     </row>
@@ -8420,15 +8607,15 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" s="37" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="37" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8441,23 +8628,23 @@
         <v>150</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8470,7 +8657,7 @@
         <v>156</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8478,15 +8665,15 @@
         <v>206</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="16" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8499,7 +8686,7 @@
         <v>181</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8507,7 +8694,7 @@
         <v>153</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8522,17 +8709,17 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
     <row r="26" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8557,17 +8744,17 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8577,17 +8764,17 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8595,35 +8782,35 @@
         <v>144</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="44" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8638,37 +8825,37 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="56" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8678,34 +8865,34 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8725,40 +8912,40 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="73" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8771,28 +8958,28 @@
         <v>148</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -8822,33 +9009,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="36.2064777327935"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="114.939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="36.5263157894737"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="115.902834008097"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="60.417004048583"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="60.9514170040486"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8860,13 +9047,13 @@
         <v>88</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8886,7 +9073,7 @@
         <v>0.075</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8901,7 +9088,7 @@
         <v>0.075</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8916,7 +9103,7 @@
         <v>0.075</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8931,7 +9118,7 @@
         <v>0.075</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8946,7 +9133,7 @@
         <v>0.075</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8961,7 +9148,7 @@
         <v>0.075</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8986,7 +9173,7 @@
         <v>0.075</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9001,7 +9188,7 @@
         <v>0.075</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9016,7 +9203,7 @@
         <v>0.075</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9031,7 +9218,7 @@
         <v>0.075</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9041,7 +9228,7 @@
         <v>0.075</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9056,7 +9243,7 @@
         <v>0.075</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9071,7 +9258,7 @@
         <v>0.075</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9086,7 +9273,7 @@
         <v>0.075</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9101,7 +9288,7 @@
         <v>0.075</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9116,7 +9303,7 @@
         <v>0.075</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9145,7 +9332,7 @@
         <v>0.064</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9160,10 +9347,10 @@
         <v>0.064</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9178,10 +9365,10 @@
         <v>0.059</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="F29" s="41" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9196,10 +9383,10 @@
         <v>0.059</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="F30" s="41" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9215,7 +9402,7 @@
         <v>0.075</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9230,7 +9417,7 @@
         <v>0.075</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9245,7 +9432,7 @@
         <v>0.075</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9260,13 +9447,13 @@
         <v>0.075</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0"/>
       <c r="B36" s="32" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="C36" s="31" t="s">
         <v>218</v>
@@ -9275,7 +9462,7 @@
         <v>0.075</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9290,7 +9477,7 @@
         <v>0.075</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9301,7 +9488,7 @@
         <v>0.075</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9316,7 +9503,7 @@
         <v>0.075</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="K39" s="27"/>
       <c r="L39" s="42"/>
@@ -9343,7 +9530,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="40" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="B40" s="32" t="s">
         <v>224</v>
@@ -9355,7 +9542,7 @@
         <v>0.075</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="K40" s="27"/>
       <c r="L40" s="42"/>
@@ -9486,32 +9673,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.2429149797571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.0931174089069"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.5182186234818"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.8137651821862"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.4574898785425"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.6315789473684"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="76.1619433198381"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.0283400809717"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -9520,10 +9707,10 @@
         <v>88</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>3</v>
@@ -9531,133 +9718,133 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="D8" s="39" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="C10" s="31" t="s">
         <v>312</v>
       </c>
-      <c r="C10" s="31" t="s">
-        <v>308</v>
-      </c>
       <c r="D10" s="39" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="D11" s="39" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="D12" s="39" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="D14" s="39" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="D15" s="39" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="D16" s="39" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9676,16 +9863,16 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>
       <c r="B21" s="32" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="D21" s="39" t="s">
         <v>144</v>
@@ -9694,10 +9881,10 @@
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1"/>
       <c r="B22" s="32" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="D22" s="39" t="s">
         <v>144</v>
@@ -9706,10 +9893,10 @@
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1"/>
       <c r="B23" s="32" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="D23" s="39" t="s">
         <v>144</v>
@@ -9717,10 +9904,10 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="32" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="D24" s="39" t="s">
         <v>144</v>
@@ -9728,10 +9915,10 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="32" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="D25" s="39" t="s">
         <v>144</v>
@@ -9743,13 +9930,13 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="D27" s="39" t="s">
         <v>144</v>
@@ -9757,10 +9944,10 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="D28" s="39" t="s">
         <v>144</v>
@@ -9768,10 +9955,10 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="D29" s="39" t="s">
         <v>144</v>
@@ -9779,10 +9966,10 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="D30" s="39" t="s">
         <v>144</v>
@@ -9790,10 +9977,10 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="D31" s="39" t="s">
         <v>144</v>
@@ -9805,16 +9992,16 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="D33" s="39"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="32" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="D34" s="39" t="s">
         <v>144</v>
@@ -9822,10 +10009,10 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="32" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="D35" s="39" t="s">
         <v>144</v>
@@ -9833,7 +10020,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>